<commit_message>
Weight measurements + minor modifications for graphs
</commit_message>
<xml_diff>
--- a/adult-DSS-exp4/adult48_weight.xlsx
+++ b/adult-DSS-exp4/adult48_weight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\adult-DSS-exp4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF4567-DA51-4922-B79C-7A15DB84B4E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D1278-3C7B-41CC-A5D2-19FA683FBC7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{597B7840-0546-4187-AEFE-CBC0766A7F04}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>33244-</t>
   </si>
@@ -33,9 +33,6 @@
     <t>26242A-398629</t>
   </si>
   <si>
-    <t>36638D</t>
-  </si>
-  <si>
     <t>27142B-402142</t>
   </si>
   <si>
@@ -87,24 +84,15 @@
     <t>23434A-397329</t>
   </si>
   <si>
-    <t>35742A</t>
-  </si>
-  <si>
     <t>33249-</t>
   </si>
   <si>
     <t>23396B-396377</t>
   </si>
   <si>
-    <t>36635A</t>
-  </si>
-  <si>
     <t>35708C</t>
   </si>
   <si>
-    <t>35747B</t>
-  </si>
-  <si>
     <t>26248A-398635</t>
   </si>
   <si>
@@ -177,18 +165,6 @@
     <t>36636B</t>
   </si>
   <si>
-    <t>35741-</t>
-  </si>
-  <si>
-    <t>35748C</t>
-  </si>
-  <si>
-    <t>33250A</t>
-  </si>
-  <si>
-    <t>35730-</t>
-  </si>
-  <si>
     <t>33278B</t>
   </si>
   <si>
@@ -226,6 +202,30 @@
   </si>
   <si>
     <t>body_weight</t>
+  </si>
+  <si>
+    <t>35764D</t>
+  </si>
+  <si>
+    <t>35763C</t>
+  </si>
+  <si>
+    <t>35761A</t>
+  </si>
+  <si>
+    <t>35762B</t>
+  </si>
+  <si>
+    <t>35760-</t>
+  </si>
+  <si>
+    <t>36646C</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>BODY_WEIGHT</t>
   </si>
 </sst>
 </file>
@@ -333,18 +333,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB0A3C2-5D06-4C72-B527-C16573CACB45}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,45 +670,54 @@
     <col min="1" max="1" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>269160</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>45385</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <f>(J$3-D2)/7</f>
         <v>11</v>
+      </c>
+      <c r="G2">
+        <v>20.2</v>
       </c>
       <c r="J2" s="1">
         <v>45453</v>
@@ -720,24 +729,33 @@
         <f>AVERAGE(F2:F25)</f>
         <v>8.797619047619051</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9">
-        <v>271387</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="M2" s="2">
+        <f>AVERAGE(G2:G25)</f>
+        <v>18.241666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>270764</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45411</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10">
-        <v>45411</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <f>(J$3-D3)/7</f>
         <v>7.2857142857142856</v>
+      </c>
+      <c r="G3">
+        <v>18.5</v>
       </c>
       <c r="J3" s="1">
         <v>45462</v>
@@ -749,958 +767,1123 @@
         <f>AVERAGE(F26:F49)</f>
         <v>8.8035714285714288</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="M3" s="2">
+        <f>AVERAGE(G26:G49)</f>
+        <v>18.920833333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>270752</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45404</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6">
-        <v>45404</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <f>(J$3-D4)/7</f>
         <v>8.2857142857142865</v>
       </c>
+      <c r="G4">
+        <v>18.100000000000001</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
         <v>270754</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8">
+        <v>45405</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10">
-        <v>45405</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="F5" s="9">
         <f>(J$3-D5)/7</f>
         <v>8.1428571428571423</v>
       </c>
+      <c r="G5">
+        <v>16.600000000000001</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>269160</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5">
         <v>45385</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f>(J$3-D6)/7</f>
         <v>11</v>
       </c>
+      <c r="G6">
+        <v>19.899999999999999</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7">
         <v>270374</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8">
+        <v>45401</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10">
-        <v>45401</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="F7" s="9">
         <f>(J$3-D7)/7</f>
         <v>8.7142857142857135</v>
       </c>
+      <c r="G7">
+        <v>17.8</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>4</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>269707</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45393</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="6">
-        <v>45393</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <f>(J$3-D8)/7</f>
         <v>9.8571428571428577</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9">
+      <c r="G8">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
         <v>270386</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="8">
+        <v>45397</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10">
-        <v>45397</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <f>(J$3-D9)/7</f>
         <v>9.2857142857142865</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="G9">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>269160</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5">
         <v>45385</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <f>(J$3-D10)/7</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9">
+      <c r="G10">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
         <v>269711</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8">
+        <v>45394</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10">
-        <v>45394</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <f>(J$3-D11)/7</f>
         <v>9.7142857142857135</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="G11">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>270388</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45400</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="6">
-        <v>45400</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <f>(J$3-D12)/7</f>
         <v>8.8571428571428577</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9">
-        <v>270758</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="G12">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7">
+        <v>270764</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="8">
         <v>45407</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="9">
         <f>(J$3-D13)/7</f>
         <v>7.8571428571428568</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="G13">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>7</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>269703</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5">
         <v>45390</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="6">
         <f>(J$3-D14)/7</f>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9">
-        <v>271387</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="G14">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7">
+        <v>270764</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="8">
         <v>45411</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="11">
+      <c r="E15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="9">
         <f>(J$3-D15)/7</f>
         <v>7.2857142857142856</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="G15">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
         <v>8</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>270388</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="5">
         <v>45400</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6">
         <f>(J$3-D16)/7</f>
         <v>8.8571428571428577</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9">
-        <v>270760</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="G16">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7">
+        <v>270764</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="8">
         <v>45409</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="11">
+      <c r="E17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9">
         <f>(J$3-D17)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="G17">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>9</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>270760</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="5">
         <v>45409</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="6">
         <f>(J$3-D18)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9">
+      <c r="G18">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7">
         <v>271387</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="C19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="8">
         <v>45411</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="11">
+      <c r="E19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="9">
         <f>(J$3-D19)/7</f>
         <v>7.2857142857142856</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="G19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>10</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>269711</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="6">
+      <c r="C20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="5">
         <v>45394</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="E20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="6">
         <f>(J$3-D20)/7</f>
         <v>9.7142857142857135</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9">
+      <c r="G20">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>10</v>
+      </c>
+      <c r="B21" s="7">
         <v>269713</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="10">
+      <c r="C21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="8">
         <v>45395</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="E21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="9">
         <f>(J$3-D21)/7</f>
         <v>9.5714285714285712</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="G21">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <v>11</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>270754</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="6">
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5">
         <v>45405</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="7">
+      <c r="E22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="6">
         <f>(J$3-D22)/7</f>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9">
+      <c r="G22">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>11</v>
+      </c>
+      <c r="B23" s="7">
         <v>270761</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="8">
         <v>45409</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="11">
+      <c r="E23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="9">
         <f>(J$3-D23)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="G23">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>12</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>270374</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="6">
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5">
         <v>45401</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="E24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="6">
         <f>(J$3-D24)/7</f>
         <v>8.7142857142857135</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9">
+      <c r="G24">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>12</v>
+      </c>
+      <c r="B25" s="7">
         <v>270761</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="10">
+      <c r="C25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="8">
         <v>45409</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="11">
+      <c r="E25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="9">
         <f>(J$3-D25)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="G25">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
         <v>13</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>269160</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="6">
+      <c r="C26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="5">
         <v>45385</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <f>(J$3-D26)/7</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9">
+      <c r="G26">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>13</v>
+      </c>
+      <c r="B27" s="7">
         <v>269709</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="10">
+      <c r="C27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="8">
         <v>45393</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="11">
+      <c r="E27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9">
         <f>(J$3-D27)/7</f>
         <v>9.8571428571428577</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="G27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <v>14</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>270388</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="5">
         <v>45400</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="7">
+      <c r="E28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="6">
         <f>(J$3-D28)/7</f>
         <v>8.8571428571428577</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9">
+      <c r="G28">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>14</v>
+      </c>
+      <c r="B29" s="7">
         <v>270754</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="10">
+      <c r="C29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="8">
         <v>45405</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="11">
+      <c r="E29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="9">
         <f>(J$3-D29)/7</f>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="G29">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <v>15</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>269160</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="6">
+      <c r="C30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="5">
         <v>45385</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <f>(J$3-D30)/7</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9">
+      <c r="G30">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>15</v>
+      </c>
+      <c r="B31" s="7">
         <v>270752</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="10">
+      <c r="C31" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="8">
         <v>45404</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="11">
+      <c r="E31" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="9">
         <f>(J$3-D31)/7</f>
         <v>8.2857142857142865</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="G31">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <v>16</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>269707</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="6">
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="5">
         <v>45393</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="7">
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="6">
         <f>(J$3-D32)/7</f>
         <v>9.8571428571428577</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9">
+      <c r="G32">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>16</v>
+      </c>
+      <c r="B33" s="7">
         <v>270374</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="10">
+      <c r="C33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="8">
         <v>45401</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="11">
+      <c r="E33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="9">
         <f>(J$3-D33)/7</f>
         <v>8.7142857142857135</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="G33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>17</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <v>270374</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="6">
+      <c r="C34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="5">
         <v>45401</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="7">
+      <c r="E34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="6">
         <f>(J$3-D34)/7</f>
         <v>8.7142857142857135</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9">
+      <c r="G34">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>17</v>
+      </c>
+      <c r="B35" s="7">
         <v>271387</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="10">
+      <c r="C35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="8">
         <v>45411</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="11">
+      <c r="E35" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="9">
         <f>(J$3-D35)/7</f>
         <v>7.2857142857142856</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="G35">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
         <v>18</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>269713</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="6">
+      <c r="C36" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="5">
         <v>45395</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="7">
+      <c r="E36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="6">
         <f>(J$3-D36)/7</f>
         <v>9.5714285714285712</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9">
+      <c r="G36">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>18</v>
+      </c>
+      <c r="B37" s="7">
         <v>270760</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="10">
+      <c r="C37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="8">
         <v>45409</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="11">
+      <c r="E37" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="9">
         <f>(J$3-D37)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="G37">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
         <v>19</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>269713</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="C38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="5">
         <v>45395</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="7">
+      <c r="E38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="6">
         <f>(J$3-D38)/7</f>
         <v>9.5714285714285712</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9">
+      <c r="G38">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>19</v>
+      </c>
+      <c r="B39" s="7">
         <v>271387</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="10">
+      <c r="C39" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="8">
         <v>45411</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="11">
+      <c r="E39" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="9">
         <f>(J$3-D39)/7</f>
         <v>7.2857142857142856</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="G39">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
         <v>20</v>
       </c>
-      <c r="B40" s="5">
-        <v>270758</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="6">
+      <c r="B40" s="7">
+        <v>270764</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5">
         <v>45407</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <f>(J$3-D40)/7</f>
         <v>7.8571428571428568</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9">
-        <v>270760</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="10">
+      <c r="G40">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>20</v>
+      </c>
+      <c r="B41" s="7">
+        <v>271389</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="8">
         <v>45409</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="11">
+      <c r="E41" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="9">
         <f>(J$3-D41)/7</f>
         <v>7.5714285714285712</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="G41">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
         <v>21</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="4">
         <v>269703</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="6">
+      <c r="C42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="5">
         <v>45390</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="7">
+      <c r="E42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="6">
         <f>(J$3-D42)/7</f>
         <v>10.285714285714286</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9">
+      <c r="G42">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>21</v>
+      </c>
+      <c r="B43" s="7">
         <v>270754</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="10">
+      <c r="C43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="8">
         <v>45405</v>
       </c>
-      <c r="E43" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="11">
+      <c r="E43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="9">
         <f>(J$3-D43)/7</f>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="G43">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
         <v>22</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="4">
         <v>269713</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D44" s="6">
+      <c r="C44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="5">
         <v>45395</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44" s="7">
+      <c r="E44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="6">
         <f>(J$3-D44)/7</f>
         <v>9.5714285714285712</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="9">
+      <c r="G44">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>22</v>
+      </c>
+      <c r="B45" s="7">
         <v>270374</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="10">
+      <c r="C45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="8">
         <v>45401</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="11">
+      <c r="E45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="9">
         <f>(J$3-D45)/7</f>
         <v>8.7142857142857135</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="G45">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
         <v>23</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>270133</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="6">
+      <c r="C46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="5">
         <v>45396</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F46" s="7">
+      <c r="E46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" s="6">
         <f>(J$3-D46)/7</f>
         <v>9.4285714285714288</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="9">
+      <c r="G46">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>23</v>
+      </c>
+      <c r="B47" s="7">
         <v>270754</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="10">
+      <c r="C47" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="8">
         <v>45405</v>
       </c>
-      <c r="E47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="11">
+      <c r="E47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="9">
         <f>(J$3-D47)/7</f>
         <v>8.1428571428571423</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="G47">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
         <v>24</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="4">
         <v>270752</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="6">
+      <c r="C48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="5">
         <v>45404</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F48" s="7">
+      <c r="E48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="6">
         <f>(J$3-D48)/7</f>
         <v>8.2857142857142865</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9">
+      <c r="G48">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>24</v>
+      </c>
+      <c r="B49" s="7">
         <v>270761</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="10">
+      <c r="C49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="8">
         <v>45409</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" s="11">
+      <c r="E49" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="9">
         <f>(J$3-D49)/7</f>
         <v>7.5714285714285712</v>
       </c>
+      <c r="G49">
+        <v>18.3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A10:A11"/>
-  </mergeCells>
+  <sortState ref="A2:G49">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>